<commit_message>
Add a few data_transform mothods
</commit_message>
<xml_diff>
--- a/ML - 2.1/result/result.xlsx
+++ b/ML - 2.1/result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/ML_Project/ML - 2.1/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751769BF-D4EE-DD4C-BC81-1992B00AA8FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38D975A-976D-3B4C-B0BC-B448EE25673F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{988CF9A7-288C-3E4E-AED1-F36208A1A063}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{988CF9A7-288C-3E4E-AED1-F36208A1A063}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,72 +31,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>default_linear_learner</t>
-  </si>
-  <si>
-    <t>default_tree_learner</t>
-  </si>
-  <si>
-    <t>kernel_ridge_learner</t>
-  </si>
-  <si>
-    <t>esn_ridge_learner</t>
-  </si>
-  <si>
-    <t>esn_kernel_ridge_learner</t>
-  </si>
-  <si>
-    <t>ws*cos(wd)</t>
-  </si>
-  <si>
-    <t>ws*sin(wd)</t>
-  </si>
-  <si>
-    <t>ws*cos(wd)-3</t>
-  </si>
-  <si>
-    <t>ws+wd</t>
-  </si>
-  <si>
-    <t>esn_linear_svr_learner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>linear_svr_learner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ws+cos(wd)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ws+sin(wd)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ws+cos(wd)-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ws+cos(wd)-6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lasso learner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ws+sin(wd)+cos(wd)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ws*sin(wd)+ws*cos(wd)</t>
+    <t>1. ws+wd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. ws+wd-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. ws+wd-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. ws+sin(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. ws+cos(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. ws+cos(wd)-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. ws+cos(wd)-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. ws+sin(wd)+cos(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. ws+sin(wd)+cos(wd)-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. ws*sin(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. ws*cos(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12. ws*cos(wd)-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13. ws*sin(wd)+ws*cos(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14. ws*sin(wd)+ws*cos(wd)-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. default_linear_learner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. default_tree_learner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. lasso learner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. linear_svr_learner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. kernel_ridge_learner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. esn_ridge_learner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. esn_kernel_ridge_learner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. esn_linear_svr_learner</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -104,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,6 +147,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -152,11 +185,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -473,285 +509,447 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDA6BDD-8D52-DF45-BD1E-82748700E3F6}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="11" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" customWidth="1"/>
+    <col min="14" max="14" width="24.83203125" customWidth="1"/>
+    <col min="15" max="15" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>0</v>
       </c>
       <c r="B2">
         <v>3.1199999999999999E-2</v>
       </c>
       <c r="C2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D2">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="E2">
         <v>2.4899999999999999E-2</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>2.4899999999999999E-2</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="H2">
+      <c r="I2">
+        <v>2.4899999999999999E-2</v>
+      </c>
+      <c r="J2">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="K2">
+        <v>6.3200000000000006E-2</v>
+      </c>
+      <c r="L2">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="I2">
-        <v>6.3200000000000006E-2</v>
-      </c>
-      <c r="J2">
+      <c r="M2">
         <v>5.9299999999999999E-2</v>
       </c>
+      <c r="N2">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="O2">
+        <v>4.5999999999999999E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>4.0300000000000002E-2</v>
       </c>
       <c r="C3">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D3">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.2099999999999999E-2</v>
+      </c>
+      <c r="F3">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="D3">
+      <c r="G3">
+        <v>0.40889999999999999</v>
+      </c>
+      <c r="H3">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="I3">
         <v>4.2099999999999999E-2</v>
       </c>
-      <c r="E3">
-        <v>0.40889999999999999</v>
-      </c>
-      <c r="F3">
-        <v>4.2299999999999997E-2</v>
-      </c>
-      <c r="H3">
+      <c r="J3">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="K3">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="L3">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="I3">
-        <v>5.9299999999999999E-2</v>
-      </c>
-      <c r="J3">
+      <c r="M3">
         <v>5.28E-2</v>
       </c>
+      <c r="N3">
+        <v>4.24E-2</v>
+      </c>
+      <c r="O3">
+        <v>4.3299999999999998E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="E4" s="1">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F4" s="1">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>3.1399999999999997E-2</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>3.15E-2</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="1">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3.15E-2</v>
+      </c>
+      <c r="K4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L4">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="I4">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="J4">
+      <c r="M4">
         <v>6.4199999999999993E-2</v>
       </c>
+      <c r="N4">
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="O4">
+        <v>4.5900000000000003E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="F5" s="1">
         <v>1.89E-2</v>
       </c>
-      <c r="D5" s="1">
-        <v>1.9800000000000002E-2</v>
-      </c>
-      <c r="E5">
+      <c r="G5">
         <v>5.9299999999999999E-2</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>5.9400000000000001E-2</v>
       </c>
-      <c r="H5">
+      <c r="I5" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2.18E-2</v>
+      </c>
+      <c r="K5">
+        <v>5.9200000000000003E-2</v>
+      </c>
+      <c r="L5">
         <v>5.9299999999999999E-2</v>
       </c>
-      <c r="I5">
-        <v>5.9200000000000003E-2</v>
-      </c>
-      <c r="J5">
+      <c r="M5">
         <v>5.9299999999999999E-2</v>
       </c>
+      <c r="N5">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="O5">
+        <v>4.3299999999999998E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>4.7800000000000002E-2</v>
       </c>
       <c r="C6">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.378</v>
+      </c>
+      <c r="E6">
+        <v>3.4099999999999998E-2</v>
+      </c>
+      <c r="F6">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D6">
-        <v>3.4099999999999998E-2</v>
-      </c>
-      <c r="E6">
+      <c r="G6">
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>3.8300000000000001E-2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
+        <v>0.03</v>
+      </c>
+      <c r="J6">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="K6">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="L6">
         <v>4.7399999999999998E-2</v>
       </c>
-      <c r="I6">
-        <v>4.5600000000000002E-2</v>
-      </c>
-      <c r="J6">
+      <c r="M6">
         <v>3.15E-2</v>
       </c>
+      <c r="N6">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="O6">
+        <v>4.2299999999999997E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>4.82E-2</v>
       </c>
       <c r="C7">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="D7">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>5.21E-2</v>
+      </c>
+      <c r="F7">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="D7">
-        <v>5.21E-2</v>
-      </c>
-      <c r="E7">
+      <c r="G7">
         <v>3.7900000000000003E-2</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.93889999999999996</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="J7">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2.58E-2</v>
+      </c>
+      <c r="L7" s="2">
         <v>2.63E-2</v>
       </c>
-      <c r="I7" s="1">
-        <v>2.58E-2</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="M7" s="2">
         <v>2.76E-2</v>
       </c>
+      <c r="N7" s="2">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="O7" s="2">
+        <v>4.2700000000000002E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>4.4200000000000003E-2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="D8">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="F8" s="1">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="D8" s="1">
-        <v>2.5700000000000001E-2</v>
-      </c>
-      <c r="E8">
+      <c r="G8">
         <v>3.8699999999999998E-2</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>3.6700000000000003E-2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
+        <v>2.4E-2</v>
+      </c>
+      <c r="J8">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="K8">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="L8">
         <v>7.0400000000000004E-2</v>
       </c>
-      <c r="I8">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="J8">
+      <c r="M8">
         <v>4.6399999999999997E-2</v>
       </c>
+      <c r="N8">
+        <v>6.3299999999999995E-2</v>
+      </c>
+      <c r="O8">
+        <v>4.4600000000000001E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
         <v>2.75E-2</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="D9">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="F9" s="1">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="D9" s="1">
-        <v>1.7100000000000001E-2</v>
-      </c>
-      <c r="E9">
+      <c r="G9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="H9">
+      <c r="I9" s="1">
+        <v>1.95E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3.61E-2</v>
+      </c>
+      <c r="K9">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="L9">
         <v>5.9400000000000001E-2</v>
       </c>
-      <c r="I9">
-        <v>5.9299999999999999E-2</v>
-      </c>
-      <c r="J9">
+      <c r="M9">
         <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="N9">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="O9">
+        <v>4.6699999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a few data_transform methods
</commit_message>
<xml_diff>
--- a/ML - 2.1/result/result.xlsx
+++ b/ML - 2.1/result/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/ML_Project/ML - 2.1/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38D975A-976D-3B4C-B0BC-B448EE25673F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0DAC47-6846-F14D-8D55-233B17854C70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{988CF9A7-288C-3E4E-AED1-F36208A1A063}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,30 +69,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9. ws+sin(wd)+cos(wd)-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10. ws*sin(wd)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11. ws*cos(wd)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12. ws*cos(wd)-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13. ws*sin(wd)+ws*cos(wd)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14. ws*sin(wd)+ws*cos(wd)-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. default_linear_learner</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,6 +98,38 @@
   </si>
   <si>
     <t>8. esn_linear_svr_learner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. ws+sin(wd)+cos(wd)-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. ws+sin(wd)+cos(wd)-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. ws*sin(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12. ws*cos(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13. ws*cos(wd)-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14. ws*sin(wd)+ws*cos(wd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15. ws*sin(wd)+ws*cos(wd)-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16. ws*sin(wd)+ws*cos(wd)-3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -509,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDA6BDD-8D52-DF45-BD1E-82748700E3F6}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="92" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -525,14 +533,16 @@
     <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
     <col min="9" max="9" width="20.1640625" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
-    <col min="11" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" customWidth="1"/>
-    <col min="14" max="14" width="24.83203125" customWidth="1"/>
-    <col min="15" max="15" width="26.5" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="12" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="17.1640625" customWidth="1"/>
+    <col min="15" max="15" width="24.83203125" customWidth="1"/>
+    <col min="16" max="16" width="26.33203125" customWidth="1"/>
+    <col min="17" max="17" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,27 +571,33 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2">
         <v>3.1199999999999999E-2</v>
@@ -608,27 +624,33 @@
         <v>2.4899999999999999E-2</v>
       </c>
       <c r="J2">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="K2">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>6.3200000000000006E-2</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>6.3299999999999995E-2</v>
-      </c>
-      <c r="M2">
-        <v>5.9299999999999999E-2</v>
       </c>
       <c r="N2">
         <v>5.9299999999999999E-2</v>
       </c>
       <c r="O2">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="P2">
         <v>4.5999999999999999E-2</v>
       </c>
+      <c r="Q2">
+        <v>4.5999999999999999E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>4.0300000000000002E-2</v>
@@ -655,27 +677,33 @@
         <v>4.2099999999999999E-2</v>
       </c>
       <c r="J3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K3">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>5.9299999999999999E-2</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>5.28E-2</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>4.24E-2</v>
       </c>
-      <c r="O3">
+      <c r="P3">
+        <v>4.3700000000000003E-2</v>
+      </c>
+      <c r="Q3">
         <v>4.3299999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>2.2800000000000001E-2</v>
@@ -701,28 +729,34 @@
       <c r="I4" s="1">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>3.15E-2</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
+        <v>3.15E-2</v>
+      </c>
+      <c r="L4">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>6.4199999999999993E-2</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>4.5900000000000003E-2</v>
       </c>
+      <c r="Q4">
+        <v>4.5900000000000003E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>2.4500000000000001E-2</v>
@@ -748,28 +782,34 @@
       <c r="I5" s="1">
         <v>0.02</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="K5" s="2">
         <v>2.18E-2</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>5.9200000000000003E-2</v>
-      </c>
-      <c r="L5">
-        <v>5.9299999999999999E-2</v>
       </c>
       <c r="M5">
         <v>5.9299999999999999E-2</v>
       </c>
       <c r="N5">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="O5">
         <v>5.9400000000000001E-2</v>
       </c>
-      <c r="O5">
+      <c r="P5">
+        <v>4.3700000000000003E-2</v>
+      </c>
+      <c r="Q5">
         <v>4.3299999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>4.7800000000000002E-2</v>
@@ -796,27 +836,33 @@
         <v>0.03</v>
       </c>
       <c r="J6">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="K6">
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>4.5600000000000002E-2</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>4.7399999999999998E-2</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>3.15E-2</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="O6">
+      <c r="P6">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="Q6">
         <v>4.2299999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>4.82E-2</v>
@@ -843,27 +889,33 @@
         <v>3.8699999999999998E-2</v>
       </c>
       <c r="J7">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="K7">
         <v>3.6400000000000002E-2</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>2.58E-2</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>2.63E-2</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>2.76E-2</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="Q7" s="2">
         <v>4.2700000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>4.4200000000000003E-2</v>
@@ -890,27 +942,33 @@
         <v>2.4E-2</v>
       </c>
       <c r="J8">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="K8">
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>7.0400000000000004E-2</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>4.6399999999999997E-2</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="O8">
+      <c r="P8" s="2">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="Q8">
         <v>4.4600000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>2.75E-2</v>
@@ -933,14 +991,14 @@
       <c r="I9" s="1">
         <v>1.95E-2</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="K9" s="2">
         <v>3.61E-2</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>5.9299999999999999E-2</v>
-      </c>
-      <c r="L9">
-        <v>5.9400000000000001E-2</v>
       </c>
       <c r="M9">
         <v>5.9400000000000001E-2</v>
@@ -949,6 +1007,12 @@
         <v>5.9400000000000001E-2</v>
       </c>
       <c r="O9">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="P9" s="2">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="Q9">
         <v>4.6699999999999998E-2</v>
       </c>
     </row>

</xml_diff>